<commit_message>
Primera versión trabajo finalizado
</commit_message>
<xml_diff>
--- a/data/bmw_50_filas.xlsx
+++ b/data/bmw_50_filas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR51"/>
+  <dimension ref="A1:AM51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,104 +551,79 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>modelo_Gran</t>
+          <t>modelo_Gran_Coupe</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>modelo_Active</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>modelo_Tourer</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>modelo_Turismo</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>modelo_Coupe</t>
         </is>
       </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_Active_Tourer</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_Gran_Tourer</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_Gran_Turismo</t>
+        </is>
+      </c>
       <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>modelo_ActiveHybrid</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>años_coche_ordinal</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_convertible</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_coupe</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_estate</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_hatchback</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_sedan</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_subcompact</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_suv</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>tipo_coche_van</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_1-3</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_11-15</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_16-20</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_21-25</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_4-6</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_7-10</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>años_coche_&gt;25</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -699,7 +674,7 @@
       <c r="P2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" t="b">
         <v>0</v>
       </c>
       <c r="R2" t="n">
@@ -742,13 +717,13 @@
         <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2" t="n">
         <v>0</v>
@@ -766,21 +741,6 @@
         <v>0</v>
       </c>
       <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,7 +791,7 @@
       <c r="P3" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" t="b">
         <v>1</v>
       </c>
       <c r="R3" t="n">
@@ -871,13 +831,13 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
@@ -895,24 +855,9 @@
         <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -965,7 +910,7 @@
       <c r="P4" t="n">
         <v>1</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" t="b">
         <v>0</v>
       </c>
       <c r="R4" t="n">
@@ -1008,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF4" t="n">
         <v>0</v>
@@ -1017,13 +962,13 @@
         <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="n">
         <v>0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4" t="n">
         <v>0</v>
@@ -1032,21 +977,6 @@
         <v>0</v>
       </c>
       <c r="AM4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1097,7 +1027,7 @@
       <c r="P5" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" t="b">
         <v>1</v>
       </c>
       <c r="R5" t="n">
@@ -1137,13 +1067,13 @@
         <v>0</v>
       </c>
       <c r="AD5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG5" t="n">
         <v>0</v>
@@ -1164,21 +1094,6 @@
         <v>0</v>
       </c>
       <c r="AM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1229,7 +1144,7 @@
       <c r="P6" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" t="b">
         <v>1</v>
       </c>
       <c r="R6" t="n">
@@ -1272,13 +1187,13 @@
         <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF6" t="n">
         <v>0</v>
       </c>
       <c r="AG6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" t="n">
         <v>0</v>
@@ -1296,21 +1211,6 @@
         <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1363,7 +1263,7 @@
       <c r="P7" t="n">
         <v>1</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" t="b">
         <v>0</v>
       </c>
       <c r="R7" t="n">
@@ -1406,13 +1306,13 @@
         <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF7" t="n">
         <v>0</v>
       </c>
       <c r="AG7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7" t="n">
         <v>0</v>
@@ -1430,21 +1330,6 @@
         <v>0</v>
       </c>
       <c r="AM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1495,7 +1380,7 @@
       <c r="P8" t="n">
         <v>1</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" t="b">
         <v>0</v>
       </c>
       <c r="R8" t="n">
@@ -1535,13 +1420,13 @@
         <v>0</v>
       </c>
       <c r="AD8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG8" t="n">
         <v>0</v>
@@ -1562,21 +1447,6 @@
         <v>0</v>
       </c>
       <c r="AM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1629,7 +1499,7 @@
       <c r="P9" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" t="b">
         <v>0</v>
       </c>
       <c r="R9" t="n">
@@ -1669,13 +1539,13 @@
         <v>0</v>
       </c>
       <c r="AD9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9" t="n">
         <v>0</v>
@@ -1696,21 +1566,6 @@
         <v>0</v>
       </c>
       <c r="AM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1761,8 +1616,8 @@
       <c r="P10" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" t="n">
-        <v>1</v>
+      <c r="Q10" t="b">
+        <v>0</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
@@ -1801,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG10" t="n">
         <v>0</v>
@@ -1828,21 +1683,6 @@
         <v>0</v>
       </c>
       <c r="AM10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1893,7 +1733,7 @@
       <c r="P11" t="n">
         <v>1</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q11" t="b">
         <v>0</v>
       </c>
       <c r="R11" t="n">
@@ -1933,13 +1773,13 @@
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG11" t="n">
         <v>0</v>
@@ -1960,21 +1800,6 @@
         <v>0</v>
       </c>
       <c r="AM11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2025,7 +1850,7 @@
       <c r="P12" t="n">
         <v>1</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="Q12" t="b">
         <v>0</v>
       </c>
       <c r="R12" t="n">
@@ -2065,13 +1890,13 @@
         <v>0</v>
       </c>
       <c r="AD12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE12" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG12" t="n">
         <v>0</v>
@@ -2092,21 +1917,6 @@
         <v>0</v>
       </c>
       <c r="AM12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2157,7 +1967,7 @@
       <c r="P13" t="n">
         <v>1</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="Q13" t="b">
         <v>0</v>
       </c>
       <c r="R13" t="n">
@@ -2197,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="AD13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG13" t="n">
         <v>0</v>
@@ -2224,21 +2034,6 @@
         <v>0</v>
       </c>
       <c r="AM13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2291,7 +2086,7 @@
       <c r="P14" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14" t="b">
         <v>1</v>
       </c>
       <c r="R14" t="n">
@@ -2334,13 +2129,13 @@
         <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF14" t="n">
         <v>0</v>
       </c>
       <c r="AG14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14" t="n">
         <v>0</v>
@@ -2358,21 +2153,6 @@
         <v>0</v>
       </c>
       <c r="AM14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2425,7 +2205,7 @@
       <c r="P15" t="n">
         <v>0</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="Q15" t="b">
         <v>1</v>
       </c>
       <c r="R15" t="n">
@@ -2468,13 +2248,13 @@
         <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15" t="n">
         <v>0</v>
       </c>
       <c r="AG15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15" t="n">
         <v>0</v>
@@ -2489,24 +2269,9 @@
         <v>0</v>
       </c>
       <c r="AL15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2559,7 +2324,7 @@
       <c r="P16" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="Q16" t="b">
         <v>0</v>
       </c>
       <c r="R16" t="n">
@@ -2599,13 +2364,13 @@
         <v>0</v>
       </c>
       <c r="AD16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG16" t="n">
         <v>0</v>
@@ -2626,21 +2391,6 @@
         <v>0</v>
       </c>
       <c r="AM16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2693,7 +2443,7 @@
       <c r="P17" t="n">
         <v>0</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="Q17" t="b">
         <v>0</v>
       </c>
       <c r="R17" t="n">
@@ -2733,13 +2483,13 @@
         <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" t="n">
         <v>0</v>
@@ -2760,21 +2510,6 @@
         <v>0</v>
       </c>
       <c r="AM17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2827,7 +2562,7 @@
       <c r="P18" t="n">
         <v>0</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Q18" t="b">
         <v>0</v>
       </c>
       <c r="R18" t="n">
@@ -2867,13 +2602,13 @@
         <v>0</v>
       </c>
       <c r="AD18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE18" t="n">
         <v>0</v>
       </c>
       <c r="AF18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG18" t="n">
         <v>0</v>
@@ -2891,24 +2626,9 @@
         <v>0</v>
       </c>
       <c r="AL18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2959,7 +2679,7 @@
       <c r="P19" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="Q19" t="b">
         <v>0</v>
       </c>
       <c r="R19" t="n">
@@ -2999,13 +2719,13 @@
         <v>0</v>
       </c>
       <c r="AD19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG19" t="n">
         <v>0</v>
@@ -3026,21 +2746,6 @@
         <v>0</v>
       </c>
       <c r="AM19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3093,7 +2798,7 @@
       <c r="P20" t="n">
         <v>1</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="Q20" t="b">
         <v>0</v>
       </c>
       <c r="R20" t="n">
@@ -3133,13 +2838,13 @@
         <v>0</v>
       </c>
       <c r="AD20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE20" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG20" t="n">
         <v>0</v>
@@ -3160,21 +2865,6 @@
         <v>0</v>
       </c>
       <c r="AM20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3225,8 +2915,8 @@
       <c r="P21" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="n">
-        <v>1</v>
+      <c r="Q21" t="b">
+        <v>0</v>
       </c>
       <c r="R21" t="n">
         <v>0</v>
@@ -3265,13 +2955,13 @@
         <v>0</v>
       </c>
       <c r="AD21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE21" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF21" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG21" t="n">
         <v>0</v>
@@ -3292,21 +2982,6 @@
         <v>0</v>
       </c>
       <c r="AM21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3359,7 +3034,7 @@
       <c r="P22" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="Q22" t="b">
         <v>0</v>
       </c>
       <c r="R22" t="n">
@@ -3399,13 +3074,13 @@
         <v>0</v>
       </c>
       <c r="AD22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE22" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG22" t="n">
         <v>0</v>
@@ -3426,21 +3101,6 @@
         <v>0</v>
       </c>
       <c r="AM22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3491,7 +3151,7 @@
       <c r="P23" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="Q23" t="b">
         <v>0</v>
       </c>
       <c r="R23" t="n">
@@ -3531,13 +3191,13 @@
         <v>0</v>
       </c>
       <c r="AD23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE23" t="n">
         <v>0</v>
       </c>
       <c r="AF23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG23" t="n">
         <v>0</v>
@@ -3555,24 +3215,9 @@
         <v>0</v>
       </c>
       <c r="AL23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3625,7 +3270,7 @@
       <c r="P24" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="Q24" t="b">
         <v>1</v>
       </c>
       <c r="R24" t="n">
@@ -3665,13 +3310,13 @@
         <v>0</v>
       </c>
       <c r="AD24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE24" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG24" t="n">
         <v>0</v>
@@ -3692,21 +3337,6 @@
         <v>0</v>
       </c>
       <c r="AM24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3757,7 +3387,7 @@
       <c r="P25" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="Q25" t="b">
         <v>0</v>
       </c>
       <c r="R25" t="n">
@@ -3800,13 +3430,13 @@
         <v>0</v>
       </c>
       <c r="AE25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF25" t="n">
         <v>0</v>
       </c>
       <c r="AG25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH25" t="n">
         <v>0</v>
@@ -3821,24 +3451,9 @@
         <v>0</v>
       </c>
       <c r="AL25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3889,8 +3504,8 @@
       <c r="P26" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="n">
-        <v>1</v>
+      <c r="Q26" t="b">
+        <v>0</v>
       </c>
       <c r="R26" t="n">
         <v>0</v>
@@ -3929,13 +3544,13 @@
         <v>0</v>
       </c>
       <c r="AD26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE26" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG26" t="n">
         <v>0</v>
@@ -3956,21 +3571,6 @@
         <v>0</v>
       </c>
       <c r="AM26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4023,7 +3623,7 @@
       <c r="P27" t="n">
         <v>1</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="Q27" t="b">
         <v>0</v>
       </c>
       <c r="R27" t="n">
@@ -4063,13 +3663,13 @@
         <v>0</v>
       </c>
       <c r="AD27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE27" t="n">
-        <v>0</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="AF27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG27" t="n">
         <v>0</v>
@@ -4090,21 +3690,6 @@
         <v>0</v>
       </c>
       <c r="AM27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4155,7 +3740,7 @@
       <c r="P28" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="Q28" t="b">
         <v>1</v>
       </c>
       <c r="R28" t="n">
@@ -4198,13 +3783,13 @@
         <v>0</v>
       </c>
       <c r="AE28" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF28" t="n">
         <v>0</v>
       </c>
       <c r="AG28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH28" t="n">
         <v>0</v>
@@ -4222,21 +3807,6 @@
         <v>0</v>
       </c>
       <c r="AM28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4287,7 +3857,7 @@
       <c r="P29" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="Q29" t="b">
         <v>1</v>
       </c>
       <c r="R29" t="n">
@@ -4327,13 +3897,13 @@
         <v>0</v>
       </c>
       <c r="AD29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE29" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG29" t="n">
         <v>0</v>
@@ -4354,21 +3924,6 @@
         <v>0</v>
       </c>
       <c r="AM29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4419,8 +3974,8 @@
       <c r="P30" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="n">
-        <v>1</v>
+      <c r="Q30" t="b">
+        <v>0</v>
       </c>
       <c r="R30" t="n">
         <v>0</v>
@@ -4459,13 +4014,13 @@
         <v>0</v>
       </c>
       <c r="AD30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE30" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG30" t="n">
         <v>0</v>
@@ -4486,21 +4041,6 @@
         <v>0</v>
       </c>
       <c r="AM30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4551,7 +4091,7 @@
       <c r="P31" t="n">
         <v>1</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="Q31" t="b">
         <v>0</v>
       </c>
       <c r="R31" t="n">
@@ -4591,13 +4131,13 @@
         <v>0</v>
       </c>
       <c r="AD31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE31" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG31" t="n">
         <v>0</v>
@@ -4618,21 +4158,6 @@
         <v>0</v>
       </c>
       <c r="AM31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4683,7 +4208,7 @@
       <c r="P32" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="Q32" t="b">
         <v>0</v>
       </c>
       <c r="R32" t="n">
@@ -4726,19 +4251,19 @@
         <v>0</v>
       </c>
       <c r="AE32" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF32" t="n">
         <v>0</v>
       </c>
       <c r="AG32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH32" t="n">
         <v>0</v>
       </c>
       <c r="AI32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ32" t="n">
         <v>0</v>
@@ -4750,21 +4275,6 @@
         <v>0</v>
       </c>
       <c r="AM32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4817,8 +4327,8 @@
       <c r="P33" t="n">
         <v>0</v>
       </c>
-      <c r="Q33" t="n">
-        <v>1</v>
+      <c r="Q33" t="b">
+        <v>0</v>
       </c>
       <c r="R33" t="n">
         <v>0</v>
@@ -4857,13 +4367,13 @@
         <v>0</v>
       </c>
       <c r="AD33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE33" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG33" t="n">
         <v>0</v>
@@ -4884,21 +4394,6 @@
         <v>0</v>
       </c>
       <c r="AM33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4949,7 +4444,7 @@
       <c r="P34" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="Q34" t="b">
         <v>0</v>
       </c>
       <c r="R34" t="n">
@@ -4989,13 +4484,13 @@
         <v>0</v>
       </c>
       <c r="AD34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE34" t="n">
         <v>0</v>
       </c>
       <c r="AF34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG34" t="n">
         <v>0</v>
@@ -5013,24 +4508,9 @@
         <v>0</v>
       </c>
       <c r="AL34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5083,7 +4563,7 @@
       <c r="P35" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="Q35" t="b">
         <v>1</v>
       </c>
       <c r="R35" t="n">
@@ -5126,13 +4606,13 @@
         <v>0</v>
       </c>
       <c r="AE35" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF35" t="n">
         <v>0</v>
       </c>
       <c r="AG35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH35" t="n">
         <v>0</v>
@@ -5150,21 +4630,6 @@
         <v>0</v>
       </c>
       <c r="AM35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5217,7 +4682,7 @@
       <c r="P36" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="n">
+      <c r="Q36" t="b">
         <v>0</v>
       </c>
       <c r="R36" t="n">
@@ -5257,13 +4722,13 @@
         <v>0</v>
       </c>
       <c r="AD36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE36" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG36" t="n">
         <v>0</v>
@@ -5284,21 +4749,6 @@
         <v>0</v>
       </c>
       <c r="AM36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5349,8 +4799,8 @@
       <c r="P37" t="n">
         <v>0</v>
       </c>
-      <c r="Q37" t="n">
-        <v>1</v>
+      <c r="Q37" t="b">
+        <v>0</v>
       </c>
       <c r="R37" t="n">
         <v>0</v>
@@ -5389,13 +4839,13 @@
         <v>0</v>
       </c>
       <c r="AD37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE37" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AF37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG37" t="n">
         <v>0</v>
@@ -5416,21 +4866,6 @@
         <v>0</v>
       </c>
       <c r="AM37" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5481,7 +4916,7 @@
       <c r="P38" t="n">
         <v>1</v>
       </c>
-      <c r="Q38" t="n">
+      <c r="Q38" t="b">
         <v>0</v>
       </c>
       <c r="R38" t="n">
@@ -5521,13 +4956,13 @@
         <v>0</v>
       </c>
       <c r="AD38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE38" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AF38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG38" t="n">
         <v>0</v>
@@ -5548,21 +4983,6 @@
         <v>0</v>
       </c>
       <c r="AM38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN38" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5613,7 +5033,7 @@
       <c r="P39" t="n">
         <v>0</v>
       </c>
-      <c r="Q39" t="n">
+      <c r="Q39" t="b">
         <v>0</v>
       </c>
       <c r="R39" t="n">
@@ -5653,13 +5073,13 @@
         <v>0</v>
       </c>
       <c r="AD39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE39" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG39" t="n">
         <v>0</v>
@@ -5680,21 +5100,6 @@
         <v>0</v>
       </c>
       <c r="AM39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ39" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5747,7 +5152,7 @@
       <c r="P40" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="n">
+      <c r="Q40" t="b">
         <v>0</v>
       </c>
       <c r="R40" t="n">
@@ -5787,13 +5192,13 @@
         <v>0</v>
       </c>
       <c r="AD40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE40" t="n">
         <v>0</v>
       </c>
       <c r="AF40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG40" t="n">
         <v>0</v>
@@ -5811,24 +5216,9 @@
         <v>0</v>
       </c>
       <c r="AL40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5881,7 +5271,7 @@
       <c r="P41" t="n">
         <v>1</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="Q41" t="b">
         <v>0</v>
       </c>
       <c r="R41" t="n">
@@ -5921,13 +5311,13 @@
         <v>0</v>
       </c>
       <c r="AD41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE41" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG41" t="n">
         <v>0</v>
@@ -5948,21 +5338,6 @@
         <v>0</v>
       </c>
       <c r="AM41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ41" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6013,7 +5388,7 @@
       <c r="P42" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="Q42" t="b">
         <v>1</v>
       </c>
       <c r="R42" t="n">
@@ -6053,13 +5428,13 @@
         <v>0</v>
       </c>
       <c r="AD42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE42" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG42" t="n">
         <v>0</v>
@@ -6080,21 +5455,6 @@
         <v>0</v>
       </c>
       <c r="AM42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6103,34 +5463,34 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.5585813165227342</v>
+        <v>0.2933186543533985</v>
       </c>
       <c r="C43" t="n">
-        <v>0.4761904761904762</v>
+        <v>0.319327731092437</v>
       </c>
       <c r="D43" t="n">
         <v>1</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
         <v>1</v>
       </c>
       <c r="J43" t="n">
-        <v>12100</v>
+        <v>15800</v>
       </c>
       <c r="K43" t="n">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
@@ -6145,7 +5505,7 @@
       <c r="P43" t="n">
         <v>1</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="Q43" t="b">
         <v>0</v>
       </c>
       <c r="R43" t="n">
@@ -6161,7 +5521,7 @@
         <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W43" t="n">
         <v>0</v>
@@ -6188,10 +5548,10 @@
         <v>0</v>
       </c>
       <c r="AE43" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG43" t="n">
         <v>0</v>
@@ -6212,21 +5572,6 @@
         <v>0</v>
       </c>
       <c r="AM43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6235,10 +5580,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.2933186543533985</v>
+        <v>0.4601839554342865</v>
       </c>
       <c r="C44" t="n">
-        <v>0.319327731092437</v>
+        <v>0.1512605042016807</v>
       </c>
       <c r="D44" t="n">
         <v>1</v>
@@ -6250,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -6259,25 +5604,25 @@
         <v>1</v>
       </c>
       <c r="J44" t="n">
-        <v>15800</v>
+        <v>8000</v>
       </c>
       <c r="K44" t="n">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="L44" t="inlineStr"/>
       <c r="M44" t="n">
         <v>1</v>
       </c>
       <c r="N44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O44" t="n">
         <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q44" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="b">
         <v>0</v>
       </c>
       <c r="R44" t="n">
@@ -6317,13 +5662,13 @@
         <v>0</v>
       </c>
       <c r="AD44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE44" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG44" t="n">
         <v>0</v>
@@ -6344,21 +5689,6 @@
         <v>0</v>
       </c>
       <c r="AM44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP44" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6367,31 +5697,31 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.4601839554342865</v>
+        <v>0.3270321126783837</v>
       </c>
       <c r="C45" t="n">
-        <v>0.1512605042016807</v>
+        <v>0.1792717086834734</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
       </c>
       <c r="E45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="K45" t="n">
         <v>0.5</v>
@@ -6409,7 +5739,7 @@
       <c r="P45" t="n">
         <v>0</v>
       </c>
-      <c r="Q45" t="n">
+      <c r="Q45" t="b">
         <v>0</v>
       </c>
       <c r="R45" t="n">
@@ -6449,13 +5779,13 @@
         <v>0</v>
       </c>
       <c r="AD45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE45" t="n">
-        <v>0</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AF45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG45" t="n">
         <v>0</v>
@@ -6476,21 +5806,6 @@
         <v>0</v>
       </c>
       <c r="AM45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ45" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6499,16 +5814,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.3270321126783837</v>
+        <v>0.02613918729951522</v>
       </c>
       <c r="C46" t="n">
-        <v>0.1792717086834734</v>
+        <v>0.123249299719888</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -6517,31 +5832,31 @@
         <v>1</v>
       </c>
       <c r="H46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>9000</v>
+        <v>24300</v>
       </c>
       <c r="K46" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="L46" t="inlineStr"/>
       <c r="M46" t="n">
         <v>1</v>
       </c>
       <c r="N46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P46" t="n">
         <v>0</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="Q46" t="b">
         <v>0</v>
       </c>
       <c r="R46" t="n">
@@ -6581,7 +5896,7 @@
         <v>0</v>
       </c>
       <c r="AD46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE46" t="n">
         <v>0</v>
@@ -6608,22 +5923,7 @@
         <v>0</v>
       </c>
       <c r="AM46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ46" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -6631,49 +5931,51 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.02613918729951522</v>
+        <v>0.3854843340445616</v>
       </c>
       <c r="C47" t="n">
-        <v>0.123249299719888</v>
+        <v>0.1092436974789916</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
       </c>
       <c r="G47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="n">
-        <v>24300</v>
+        <v>2600</v>
       </c>
       <c r="K47" t="n">
         <v>0.375</v>
       </c>
-      <c r="L47" t="inlineStr"/>
+      <c r="L47" t="n">
+        <v>0.08721618492121141</v>
+      </c>
       <c r="M47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N47" t="n">
         <v>0</v>
       </c>
       <c r="O47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q47" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q47" t="b">
         <v>0</v>
       </c>
       <c r="R47" t="n">
@@ -6716,10 +6018,10 @@
         <v>0</v>
       </c>
       <c r="AE47" t="n">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AF47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG47" t="n">
         <v>0</v>
@@ -6734,27 +6036,12 @@
         <v>0</v>
       </c>
       <c r="AK47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6763,10 +6050,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.3854843340445616</v>
+        <v>0.04238452180055728</v>
       </c>
       <c r="C48" t="n">
-        <v>0.1092436974789916</v>
+        <v>0.1932773109243697</v>
       </c>
       <c r="D48" t="n">
         <v>1</v>
@@ -6778,25 +6065,25 @@
         <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>2600</v>
+        <v>21400</v>
       </c>
       <c r="K48" t="n">
         <v>0.375</v>
       </c>
       <c r="L48" t="n">
-        <v>0.08721618492121141</v>
+        <v>0.04029017402290418</v>
       </c>
       <c r="M48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N48" t="n">
         <v>0</v>
@@ -6805,10 +6092,10 @@
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q48" t="n">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Q48" t="b">
+        <v>1</v>
       </c>
       <c r="R48" t="n">
         <v>0</v>
@@ -6847,16 +6134,16 @@
         <v>0</v>
       </c>
       <c r="AD48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE48" t="n">
-        <v>0</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF48" t="n">
         <v>0</v>
       </c>
       <c r="AG48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH48" t="n">
         <v>0</v>
@@ -6874,21 +6161,6 @@
         <v>0</v>
       </c>
       <c r="AM48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ48" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6897,13 +6169,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.04238452180055728</v>
+        <v>0.1027514825287779</v>
       </c>
       <c r="C49" t="n">
         <v>0.1932773109243697</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -6912,23 +6184,21 @@
         <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="n">
-        <v>21400</v>
+        <v>26200</v>
       </c>
       <c r="K49" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0.04029017402290418</v>
-      </c>
+        <v>0.125</v>
+      </c>
+      <c r="L49" t="inlineStr"/>
       <c r="M49" t="n">
         <v>1</v>
       </c>
@@ -6941,7 +6211,7 @@
       <c r="P49" t="n">
         <v>0</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="Q49" t="b">
         <v>1</v>
       </c>
       <c r="R49" t="n">
@@ -6984,13 +6254,13 @@
         <v>0</v>
       </c>
       <c r="AE49" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF49" t="n">
         <v>0</v>
       </c>
       <c r="AG49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH49" t="n">
         <v>0</v>
@@ -7008,21 +6278,6 @@
         <v>0</v>
       </c>
       <c r="AM49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP49" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ49" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7031,19 +6286,19 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.1027514825287779</v>
+        <v>0.303020413558916</v>
       </c>
       <c r="C50" t="n">
-        <v>0.1932773109243697</v>
+        <v>0.09523809523809523</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -7052,20 +6307,22 @@
         <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
-        <v>26200</v>
+        <v>8400</v>
       </c>
       <c r="K50" t="n">
-        <v>0.125</v>
-      </c>
-      <c r="L50" t="inlineStr"/>
+        <v>0.375</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.197448750866039</v>
+      </c>
       <c r="M50" t="n">
         <v>1</v>
       </c>
       <c r="N50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O50" t="n">
         <v>0</v>
@@ -7073,8 +6330,8 @@
       <c r="P50" t="n">
         <v>0</v>
       </c>
-      <c r="Q50" t="n">
-        <v>1</v>
+      <c r="Q50" t="b">
+        <v>0</v>
       </c>
       <c r="R50" t="n">
         <v>0</v>
@@ -7116,13 +6373,13 @@
         <v>0</v>
       </c>
       <c r="AE50" t="n">
-        <v>1</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="AF50" t="n">
         <v>0</v>
       </c>
       <c r="AG50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH50" t="n">
         <v>0</v>
@@ -7140,21 +6397,6 @@
         <v>0</v>
       </c>
       <c r="AM50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP50" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ50" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7163,22 +6405,22 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.303020413558916</v>
+        <v>0.1056349519456189</v>
       </c>
       <c r="C51" t="n">
-        <v>0.09523809523809523</v>
+        <v>0.1092436974789916</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
         <v>1</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51" t="n">
         <v>0</v>
@@ -7187,27 +6429,25 @@
         <v>0</v>
       </c>
       <c r="J51" t="n">
-        <v>8400</v>
+        <v>17100</v>
       </c>
       <c r="K51" t="n">
         <v>0.375</v>
       </c>
-      <c r="L51" t="n">
-        <v>0.197448750866039</v>
-      </c>
+      <c r="L51" t="inlineStr"/>
       <c r="M51" t="n">
         <v>1</v>
       </c>
       <c r="N51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P51" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="Q51" t="b">
         <v>0</v>
       </c>
       <c r="R51" t="n">
@@ -7250,13 +6490,13 @@
         <v>0</v>
       </c>
       <c r="AE51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF51" t="n">
         <v>0</v>
       </c>
       <c r="AG51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH51" t="n">
         <v>0</v>
@@ -7274,21 +6514,6 @@
         <v>0</v>
       </c>
       <c r="AM51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AO51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP51" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ51" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR51" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>